<commit_message>
Enhance student import functionality by adding unique UID validation and improving date of birth handling. Update sidebar for device management access and initialize variables in the teacher index page for better data handling.
</commit_message>
<xml_diff>
--- a/assets/format_data_guru.xlsx
+++ b/assets/format_data_guru.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e5b5e5968ba41335/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\absensi_sekolah\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{DF4C92A6-A589-4EDE-BD89-B529ECC33179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA69EEF1-7DD0-434D-938B-303D9D200777}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7DE558-01BE-458C-8002-0CE6F0D91BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{B37E9E71-DBD6-4565-B902-9011B4B20F74}"/>
+    <workbookView xWindow="372" yWindow="372" windowWidth="23016" windowHeight="12360" xr2:uid="{B37E9E71-DBD6-4565-B902-9011B4B20F74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,63 +35,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
-  <si>
-    <t>Laki-Laki</t>
-  </si>
-  <si>
-    <t>$2y$10$x7xWgiXMLwF/Rq4oH6Lpz.Jt1jzM5a.q8jUamJ.K4qbyXkgtdoELi</t>
-  </si>
-  <si>
-    <t>guru</t>
-  </si>
-  <si>
-    <t>nama_guru</t>
-  </si>
-  <si>
-    <t>nip</t>
-  </si>
-  <si>
-    <t>jenis_kelamin</t>
-  </si>
-  <si>
-    <t>tanggal_lahir</t>
-  </si>
-  <si>
-    <t>alamat</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>mjl</t>
-  </si>
-  <si>
-    <t>Guru_A</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>Guru_B</t>
-  </si>
-  <si>
-    <t>Guru_C</t>
-  </si>
-  <si>
-    <t>Guru_D</t>
-  </si>
-  <si>
-    <t>Guru_E</t>
-  </si>
-  <si>
-    <t>Guru_F</t>
-  </si>
-  <si>
-    <t>Guru_G</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>NIP</t>
+  </si>
+  <si>
+    <t>Nama Guru</t>
+  </si>
+  <si>
+    <t>Jenis Kelamin</t>
+  </si>
+  <si>
+    <t>Tanggal Lahir</t>
+  </si>
+  <si>
+    <t>Alamat</t>
+  </si>
+  <si>
+    <t>Budi Santoso</t>
+  </si>
+  <si>
+    <t>Laki-laki</t>
+  </si>
+  <si>
+    <t>Jl. Merdeka No. 10, Jakarta</t>
   </si>
 </sst>
 </file>
@@ -151,6 +118,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -167,10 +202,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="C0C0C0"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="191919"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -459,214 +494,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16FF389A-954C-45E9-BA8E-71FED8F92499}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="59.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>12345678901</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D2" s="2">
+        <v>29356</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>12345678</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>37147</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
-        <v>12345678</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>37148</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <v>12345679</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>37149</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>12345680</v>
-      </c>
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>37150</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6">
-        <v>12345681</v>
-      </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>37151</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7">
-        <v>12345682</v>
-      </c>
-      <c r="C7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>37152</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8">
-        <v>12345683</v>
-      </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>37153</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="D13" s="2"/>
     </row>

</xml_diff>

<commit_message>
Add WhatsApp notification functionality for attendance alerts, including late and absence notifications for both teachers and students. Implemented phone number formatting and logging for message status. Enhanced user management by adding phone number fields in user forms and updating database interactions for user creation and editing. This update improves communication and user experience in attendance management.
</commit_message>
<xml_diff>
--- a/assets/format_data_guru.xlsx
+++ b/assets/format_data_guru.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\absensi_sekolah\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7DE558-01BE-458C-8002-0CE6F0D91BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56759E8-98BA-460F-890A-A3341EFEC299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="372" yWindow="372" windowWidth="23016" windowHeight="12360" xr2:uid="{B37E9E71-DBD6-4565-B902-9011B4B20F74}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12360" xr2:uid="{B37E9E71-DBD6-4565-B902-9011B4B20F74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>NIP</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Jl. Merdeka No. 10, Jakarta</t>
+  </si>
+  <si>
+    <t>Phone</t>
   </si>
 </sst>
 </file>
@@ -108,84 +111,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -202,10 +139,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="C0C0C0"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="191919"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -494,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16FF389A-954C-45E9-BA8E-71FED8F92499}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,10 +444,10 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -526,8 +463,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>12345678901</v>
       </c>
@@ -543,40 +483,43 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="4">
+        <v>628514569875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="D13" s="2"/>
     </row>

</xml_diff>